<commit_message>
Sampeld Damjanovic alkaline again
Sampled the alkaline polarisation curve again since I got negative CI, still do, so I will consider sampling them again
</commit_message>
<xml_diff>
--- a/Data/Alkaline/Damjanovic_alkaline_polarisation.xlsx
+++ b/Data/Alkaline/Damjanovic_alkaline_polarisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/pekarste_ntnu_no/Documents/Dokumenter/NTNU/V2023/Numerics/Degradation/Data/Alkaline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{F6531480-0026-4EBE-8340-50AF42894AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C15966C-69BA-45B1-8BCA-52DD56504F34}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{F6531480-0026-4EBE-8340-50AF42894AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B62D5E61-F5E6-4457-9F8F-FF5CD1F5CA4E}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="3375" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plot-data (2)" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>log(i) - [A/cm^-2]</t>
+    <t>E - [V vs HE]</t>
   </si>
   <si>
-    <t>E - [V vs HE]</t>
+    <t>i - [A/cm^-2]</t>
   </si>
 </sst>
 </file>
@@ -580,6 +580,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -882,7 +886,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -892,10 +896,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>